<commit_message>
updated endpoint /api/user/login for all users
changed the endpoint to /api/user/login and tested. Test suit: test/user-login.test.js
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFDD064-3461-42B0-BA8A-AECF77DD26F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2042082-8C9C-4B2A-A969-71B37420FC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>route</t>
   </si>
@@ -62,9 +62,6 @@
     <t>all users</t>
   </si>
   <si>
-    <t>register for the course</t>
-  </si>
-  <si>
     <t>public</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>to change the main route to /api</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -147,6 +141,21 @@
   </si>
   <si>
     <t>Team member</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>tested with jest and supertest. Test suit: test/user-login.test.js</t>
+  </si>
+  <si>
+    <t>finalize student schema - merging student and applicant</t>
+  </si>
+  <si>
+    <t>registration for course</t>
+  </si>
+  <si>
+    <t>end point is /api/user/login now</t>
   </si>
 </sst>
 </file>
@@ -468,7 +477,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,13 +499,13 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -516,13 +525,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1">
         <v>45552</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -530,16 +539,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>45552</v>
@@ -547,30 +556,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>45552</v>
@@ -578,19 +587,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1">
         <v>45552</v>
@@ -598,97 +607,97 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -698,29 +707,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F58C10-3476-4602-99B7-4DBA48A5DFA4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,7 +740,24 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45554</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creation of super admin and related middleware
Super admin gets created automatically when server starts for the first time. Route access middleware updated to allow different levels of access.
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370F122-DD76-476F-9736-651AED9F0BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B8268B-F30A-458E-908C-ACCEE173D4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>route</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>completed on</t>
+  </si>
+  <si>
+    <t>Test suite</t>
+  </si>
+  <si>
+    <t>user-login.test.js</t>
   </si>
 </sst>
 </file>
@@ -520,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A29CE7-394B-468D-92AA-4C33F837E631}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +562,11 @@
       <c r="I1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -585,8 +594,11 @@
       <c r="I2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -609,7 +621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -635,7 +647,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>23</v>
       </c>
@@ -643,7 +655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -663,7 +675,7 @@
         <v>45552</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -683,7 +695,7 @@
         <v>45552</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -694,7 +706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -708,7 +720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -716,7 +728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -724,7 +736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -735,7 +747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -749,7 +761,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>22</v>
       </c>
@@ -757,7 +769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -765,7 +777,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -787,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F58C10-3476-4602-99B7-4DBA48A5DFA4}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -854,6 +866,7 @@
       <c r="C4" t="s">
         <v>56</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -864,7 +877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E1916-ECF3-4CE4-A96F-A40898F6C690}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
test /api/user/add to add a new admin
/api/user/add endpoint adds a new admin user. Test suite: test/user-add.test.js
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A7FE3B-4C5D-42D0-A20D-36F6B47F02A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C622E2C-AEE8-4533-8730-8AD84734E814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>route</t>
   </si>
@@ -159,9 +159,6 @@
     <t>current task</t>
   </si>
   <si>
-    <t>creating route and controller for adding user</t>
-  </si>
-  <si>
     <t>/api/user/add</t>
   </si>
   <si>
@@ -208,6 +205,21 @@
   </si>
   <si>
     <t>finalize student schema - merged student and applicant</t>
+  </si>
+  <si>
+    <t>Wrote and tested /api/user/add route to add admin user</t>
+  </si>
+  <si>
+    <t>test cases for faculty have to be included</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>admin or super admin can create a new admin</t>
+  </si>
+  <si>
+    <t>user-add.test.js</t>
   </si>
 </sst>
 </file>
@@ -528,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A29CE7-394B-468D-92AA-4C33F837E631}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +575,7 @@
         <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -595,7 +607,7 @@
         <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -615,10 +627,10 @@
         <v>45552</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -635,16 +647,19 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1">
-        <v>45553</v>
+        <v>45555</v>
       </c>
       <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
-        <v>44</v>
+      <c r="J4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -653,6 +668,15 @@
       </c>
       <c r="D5" t="s">
         <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45555</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -797,17 +821,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F58C10-3476-4602-99B7-4DBA48A5DFA4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -827,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -841,10 +865,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,10 +879,24 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45555</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -878,19 +916,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -904,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1">
         <v>45560</v>

</xml_diff>

<commit_message>
modifications to include additional admin details
Included admin sub schema with details like hireDate, salary, etc.
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C622E2C-AEE8-4533-8730-8AD84734E814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDEC033-6A42-4BF5-9DFC-F026B93DADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>route</t>
   </si>
@@ -135,21 +135,12 @@
     <t>tested with jest and supertest. Test suit: test/user-login.test.js</t>
   </si>
   <si>
-    <t>registration for course</t>
-  </si>
-  <si>
-    <t>changes required</t>
-  </si>
-  <si>
     <t>Endpoint</t>
   </si>
   <si>
     <t>/api/user/login</t>
   </si>
   <si>
-    <t>login will now return data according to polymorphic model</t>
-  </si>
-  <si>
     <t>add admin user</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>Wrote and tested /api/user/add route to add admin user</t>
   </si>
   <si>
-    <t>test cases for faculty have to be included</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -220,6 +208,27 @@
   </si>
   <si>
     <t>user-add.test.js</t>
+  </si>
+  <si>
+    <t>to check option of cookies and logout</t>
+  </si>
+  <si>
+    <t>/get</t>
+  </si>
+  <si>
+    <t>Wrote and tested /api/user/add route to add faculty</t>
+  </si>
+  <si>
+    <t>register a new user to course</t>
+  </si>
+  <si>
+    <t>Tested with jest and supertest. api doc to be created.</t>
+  </si>
+  <si>
+    <t>stand alone testing done. Yet to perform integration with department and subject models.</t>
+  </si>
+  <si>
+    <t>admin or super admin can create a new faculty (dependencies: valid departmentId and subjectId - to be tested)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,10 +581,10 @@
         <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -595,19 +604,19 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45556</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1">
-        <v>45553</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -618,7 +627,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -627,10 +636,10 @@
         <v>45552</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -641,25 +650,25 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1">
         <v>45555</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -667,21 +676,30 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1">
-        <v>45555</v>
+        <v>45556</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -821,17 +839,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F58C10-3476-4602-99B7-4DBA48A5DFA4}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -851,7 +869,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -865,10 +883,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,10 +911,24 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45556</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -916,19 +948,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -942,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>45560</v>

</xml_diff>

<commit_message>
/api/user/add tested with dependencies
/api/user/add now creates Admin, and Faculty belonging to a valid department in the database. Test suite user-add.test.js updated.
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDEC033-6A42-4BF5-9DFC-F026B93DADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24990C0-A693-4D11-A0BE-B9ECB806423A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>route</t>
   </si>
@@ -225,10 +225,7 @@
     <t>Tested with jest and supertest. api doc to be created.</t>
   </si>
   <si>
-    <t>stand alone testing done. Yet to perform integration with department and subject models.</t>
-  </si>
-  <si>
-    <t>admin or super admin can create a new faculty (dependencies: valid departmentId and subjectId - to be tested)</t>
+    <t>Admin or SuperAdmin can create a new faculty</t>
   </si>
 </sst>
 </file>
@@ -550,7 +547,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +685,7 @@
         <v>45556</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
         <v>40</v>
@@ -842,7 +839,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +925,7 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
/api/user/login works for new User model
Also moved the login functionality to a. separate fil under controllers/user/login.js. Two other test cases included for invalid login attempts. Test suite: user-login.test.js
</commit_message>
<xml_diff>
--- a/backend/project-status.xlsx
+++ b/backend/project-status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashish Mungmode\Documents\GitHub\univercity-manajment-system\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Learn\Web Development\New with React and Node\Projects\Project-final\univercity-manajment-system\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD1CC15-83D0-4A88-9F1A-73177DDE837F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF9FCC-39DD-421A-B19F-F5880A943155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t>route</t>
   </si>
@@ -210,9 +210,6 @@
     <t>user-add.test.js</t>
   </si>
   <si>
-    <t>to check option of cookies and logout</t>
-  </si>
-  <si>
     <t>/get</t>
   </si>
   <si>
@@ -253,6 +250,24 @@
   </si>
   <si>
     <t>Superadmin and admin can delete department by id</t>
+  </si>
+  <si>
+    <t>login tested for all users</t>
+  </si>
+  <si>
+    <t>/logout</t>
+  </si>
+  <si>
+    <t>logout user from the system</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>login tested with new User model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to check best technique to use with JWT </t>
   </si>
 </sst>
 </file>
@@ -572,18 +587,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A29CE7-394B-468D-92AA-4C33F837E631}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +630,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -632,13 +647,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1">
-        <v>45556</v>
+        <v>45558</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
@@ -647,64 +662,61 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45558</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <v>45552</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="1">
-        <v>45555</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -713,10 +725,10 @@
         <v>57</v>
       </c>
       <c r="G5" s="1">
-        <v>45556</v>
+        <v>45555</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
         <v>40</v>
@@ -725,35 +737,41 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1">
-        <v>45552</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>45556</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -765,138 +783,158 @@
         <v>45552</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45552</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>66</v>
-      </c>
       <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="2">
-        <v>45556</v>
-      </c>
-      <c r="H13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45556</v>
+      </c>
+      <c r="H14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="1">
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1">
         <v>45557</v>
       </c>
-      <c r="H16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="H17" t="s">
         <v>73</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -907,15 +945,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F58C10-3476-4602-99B7-4DBA48A5DFA4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -929,7 +967,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45552</v>
       </c>
@@ -943,7 +981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45553</v>
       </c>
@@ -957,7 +995,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45553</v>
       </c>
@@ -971,7 +1009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45555</v>
       </c>
@@ -982,10 +1020,10 @@
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45556</v>
       </c>
@@ -993,10 +1031,24 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45558</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1012,9 +1064,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1034,7 +1086,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45553</v>
       </c>
@@ -1059,7 +1111,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>